<commit_message>
Added TCs-CreditHold, InvoiceFromSitemap.Updated SO fulfillment TCs to reduce execution time.
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SYDATA.xlsx
+++ b/templates/AutomationOrg/SYDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5412B327-3557-4904-B5D8-814DC858943C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D761729-2F6A-4093-B02F-543F660283EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="761" firstSheet="30" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20505" yWindow="60" windowWidth="28710" windowHeight="10890" tabRatio="761" firstSheet="6" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -1733,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C02362-B38D-4703-8703-8411DD765CC8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,7 +1755,7 @@
         <v>44</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1880,7 +1880,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1901,7 +1901,7 @@
         <v>49</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1914,7 +1914,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,7 +1935,7 @@
         <v>50</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1948,7 +1948,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1966,7 +1966,7 @@
         <v>51</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1979,7 +1979,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2000,7 +2000,7 @@
         <v>52</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>71</v>
@@ -2015,7 +2015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502F24E3-35CE-4D20-B93D-E042852331C2}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>

</xml_diff>